<commit_message>
se actualizo los campos
</commit_message>
<xml_diff>
--- a/PEAJES.xlsx
+++ b/PEAJES.xlsx
@@ -1,133 +1,85 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\GIT\linea-amarilla-bajar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C720F23-65AE-4838-87C2-8F96CA8B02BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DB82B2-8173-4C56-BEF7-35589AFB10AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="972" windowWidth="17280" windowHeight="9108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="A" sheetId="1" r:id="rId1"/>
+    <sheet name="set2023" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
-  <si>
-    <t>21.07.2023</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+  <si>
+    <t>28.08.2023</t>
   </si>
   <si>
     <t>LIMA EXPRESA S.A.C.</t>
   </si>
   <si>
-    <t>03.08.2023</t>
-  </si>
-  <si>
-    <t>04.08.2023</t>
-  </si>
-  <si>
-    <t>07.08.2023</t>
-  </si>
-  <si>
-    <t>10.08.2023</t>
-  </si>
-  <si>
-    <t>14.08.2023</t>
-  </si>
-  <si>
-    <t>15.08.2023</t>
-  </si>
-  <si>
-    <t>17.08.2023</t>
-  </si>
-  <si>
-    <t>18.08.2023</t>
+    <t>19.09.2023</t>
+  </si>
+  <si>
+    <t>29.08.2023</t>
+  </si>
+  <si>
+    <t>05.09.2023</t>
+  </si>
+  <si>
+    <t>06.09.2023</t>
+  </si>
+  <si>
+    <t>14.09.2023</t>
+  </si>
+  <si>
+    <t>18.09.2023</t>
+  </si>
+  <si>
+    <t>COMPAÑIA FOOD RETAIL S.A.C.</t>
   </si>
   <si>
     <t>F260</t>
   </si>
   <si>
-    <t>357877</t>
-  </si>
-  <si>
     <t>F751</t>
   </si>
   <si>
-    <t>2002010</t>
-  </si>
-  <si>
     <t>F158</t>
   </si>
   <si>
-    <t>337279</t>
-  </si>
-  <si>
-    <t>F155</t>
-  </si>
-  <si>
-    <t>3600978</t>
+    <t>F261</t>
+  </si>
+  <si>
+    <t>F651</t>
+  </si>
+  <si>
+    <t>F255</t>
+  </si>
+  <si>
+    <t>F159</t>
+  </si>
+  <si>
+    <t>F152</t>
   </si>
   <si>
     <t>F257</t>
   </si>
   <si>
-    <t>1020195</t>
-  </si>
-  <si>
-    <t>F162</t>
-  </si>
-  <si>
-    <t>378906</t>
-  </si>
-  <si>
-    <t>F259</t>
-  </si>
-  <si>
-    <t>293479</t>
-  </si>
-  <si>
-    <t>F651</t>
-  </si>
-  <si>
-    <t>2220136</t>
-  </si>
-  <si>
-    <t>364045</t>
-  </si>
-  <si>
-    <t>364051</t>
-  </si>
-  <si>
-    <t>F261</t>
-  </si>
-  <si>
-    <t>134796</t>
-  </si>
-  <si>
-    <t>135003</t>
-  </si>
-  <si>
-    <t>364846</t>
-  </si>
-  <si>
-    <t>F161</t>
-  </si>
-  <si>
-    <t>136192</t>
-  </si>
-  <si>
-    <t>F258</t>
-  </si>
-  <si>
-    <t>661705</t>
+    <t>F160</t>
+  </si>
+  <si>
+    <t>FA17</t>
   </si>
 </sst>
 </file>
@@ -611,8 +563,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -934,21 +887,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C1" sqref="C1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="17" width="46" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -956,10 +903,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C1" s="1">
+        <v>367658</v>
       </c>
       <c r="D1">
         <v>6.6</v>
@@ -967,11 +914,8 @@
       <c r="E1">
         <v>20523621212</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
-      </c>
-      <c r="G1">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -979,10 +923,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2024734</v>
       </c>
       <c r="D2">
         <v>6.6</v>
@@ -990,22 +934,19 @@
       <c r="E2">
         <v>20523621212</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>1</v>
-      </c>
-      <c r="G2">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>344693</v>
       </c>
       <c r="D3">
         <v>6.6</v>
@@ -1013,22 +954,19 @@
       <c r="E3">
         <v>20523621212</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>1</v>
-      </c>
-      <c r="G3">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>141683</v>
       </c>
       <c r="D4">
         <v>6.6</v>
@@ -1036,11 +974,8 @@
       <c r="E4">
         <v>20523621212</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>1</v>
-      </c>
-      <c r="G4">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1048,10 +983,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2232357</v>
       </c>
       <c r="D5">
         <v>6.6</v>
@@ -1059,22 +994,19 @@
       <c r="E5">
         <v>20523621212</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>1</v>
-      </c>
-      <c r="G5">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3399744</v>
       </c>
       <c r="D6">
         <v>6.6</v>
@@ -1082,11 +1014,8 @@
       <c r="E6">
         <v>20523621212</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>1</v>
-      </c>
-      <c r="G6">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1094,10 +1023,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2081760</v>
       </c>
       <c r="D7">
         <v>6.6</v>
@@ -1105,22 +1034,19 @@
       <c r="E7">
         <v>20523621212</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>1</v>
-      </c>
-      <c r="G7">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2087717</v>
       </c>
       <c r="D8">
         <v>6.6</v>
@@ -1128,22 +1054,19 @@
       <c r="E8">
         <v>20523621212</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>1</v>
-      </c>
-      <c r="G8">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3095548</v>
       </c>
       <c r="D9">
         <v>6.6</v>
@@ -1151,22 +1074,19 @@
       <c r="E9">
         <v>20523621212</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>1</v>
-      </c>
-      <c r="G9">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1043782</v>
       </c>
       <c r="D10">
         <v>6.6</v>
@@ -1174,22 +1094,19 @@
       <c r="E10">
         <v>20523621212</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>1</v>
-      </c>
-      <c r="G10">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1172087</v>
       </c>
       <c r="D11">
         <v>6.6</v>
@@ -1197,103 +1114,28 @@
       <c r="E11">
         <v>20523621212</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>1</v>
-      </c>
-      <c r="G11">
-        <v>20100152356</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="1">
+        <v>155632</v>
       </c>
       <c r="D12">
-        <v>6.6</v>
+        <v>226.56</v>
       </c>
       <c r="E12">
-        <v>20523621212</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>20100152356</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+        <v>20608300393</v>
+      </c>
+      <c r="G12" t="s">
         <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13">
-        <v>6.6</v>
-      </c>
-      <c r="E13">
-        <v>20523621212</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>20100152356</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14">
-        <v>6.6</v>
-      </c>
-      <c r="E14">
-        <v>20523621212</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>20100152356</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15">
-        <v>6.6</v>
-      </c>
-      <c r="E15">
-        <v>20523621212</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>20100152356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>